<commit_message>
Jos nesto malo dodala
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="83">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -194,30 +194,6 @@
     <t>[ If yes, please describe the third party and their contributions]</t>
   </si>
   <si>
-    <t>WP1-</t>
-  </si>
-  <si>
-    <t>WP2-</t>
-  </si>
-  <si>
-    <t>WP3-</t>
-  </si>
-  <si>
-    <t>WP4-</t>
-  </si>
-  <si>
-    <t>WP5-</t>
-  </si>
-  <si>
-    <t>WP6-</t>
-  </si>
-  <si>
-    <t>WP7-</t>
-  </si>
-  <si>
-    <t>WP8-</t>
-  </si>
-  <si>
     <t>WP9-</t>
   </si>
   <si>
@@ -285,6 +261,60 @@
   </si>
   <si>
     <t>WP1</t>
+  </si>
+  <si>
+    <t>WP2</t>
+  </si>
+  <si>
+    <t>WP3</t>
+  </si>
+  <si>
+    <t>WP4</t>
+  </si>
+  <si>
+    <t>WP5</t>
+  </si>
+  <si>
+    <t>WP6</t>
+  </si>
+  <si>
+    <t>WP7</t>
+  </si>
+  <si>
+    <t>WP8</t>
+  </si>
+  <si>
+    <t>WP1-  Analiza korisničkih zahteva</t>
+  </si>
+  <si>
+    <t>WP2- Realizacija neophodnog harvdera</t>
+  </si>
+  <si>
+    <t>WP3- Modelovanje sistema</t>
+  </si>
+  <si>
+    <t>WP4-  Implementacija veb i mobilne aplikacije</t>
+  </si>
+  <si>
+    <t>WP5- Integracija sistema</t>
+  </si>
+  <si>
+    <t>WP6- Testiranje</t>
+  </si>
+  <si>
+    <t>WP7- Evaluacija i disiminacija</t>
+  </si>
+  <si>
+    <t>WP8- Upravljanje projektom</t>
+  </si>
+  <si>
+    <t>Smart Companion</t>
+  </si>
+  <si>
+    <t>Elektrotehnički fakultet Univerziteta u Beogradu</t>
+  </si>
+  <si>
+    <t>ETF</t>
   </si>
 </sst>
 </file>
@@ -639,7 +669,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -742,6 +772,52 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -762,56 +838,20 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1210,8 +1250,8 @@
   </sheetPr>
   <dimension ref="A1:T40"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7:I7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1223,7 +1263,8 @@
     <col min="5" max="5" width="5.5546875" customWidth="1"/>
     <col min="6" max="8" width="5.21875" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="13" width="14.21875" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" customWidth="1"/>
+    <col min="11" max="13" width="14.21875" customWidth="1"/>
     <col min="14" max="14" width="15.21875" customWidth="1"/>
     <col min="15" max="19" width="14.21875" customWidth="1"/>
   </cols>
@@ -1234,65 +1275,71 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="49"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65"/>
+      <c r="I3" s="65"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D4" s="2"/>
-      <c r="E4" s="50" t="s">
+      <c r="E4" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="3"/>
-      <c r="L4" s="51" t="s">
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="67" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="51"/>
-      <c r="N4" s="51"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D5" s="2"/>
-      <c r="E5" s="50" t="s">
+      <c r="E5" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="3"/>
-      <c r="L5" s="51" t="s">
+      <c r="F5" s="67"/>
+      <c r="G5" s="67"/>
+      <c r="H5" s="67"/>
+      <c r="I5" s="67"/>
+      <c r="J5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="67" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="51"/>
-      <c r="N5" s="51"/>
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="D6" s="2"/>
-      <c r="E6" s="50" t="s">
+      <c r="E6" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="3"/>
-      <c r="L6" s="51" t="s">
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="L6" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="51"/>
-      <c r="N6" s="51"/>
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1302,19 +1349,19 @@
       <c r="Q6" s="6"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="67" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
       <c r="J7" s="3"/>
-      <c r="L7" s="51" t="s">
+      <c r="L7" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="51"/>
-      <c r="N7" s="51"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
@@ -1325,61 +1372,61 @@
     </row>
     <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="10" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="52" t="s">
+      <c r="A10" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="53"/>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="53"/>
-      <c r="Q10" s="53"/>
-      <c r="R10" s="53"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+      <c r="R10" s="69"/>
       <c r="S10" s="8"/>
     </row>
     <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D12" s="54" t="s">
+      <c r="D12" s="70" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="54"/>
-      <c r="F12" s="54"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="55" t="s">
+      <c r="E12" s="70"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="70"/>
+      <c r="H12" s="70"/>
+      <c r="I12" s="70"/>
+      <c r="J12" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="55"/>
-      <c r="L12" s="55"/>
-      <c r="M12" s="55"/>
-      <c r="N12" s="55"/>
-      <c r="O12" s="55"/>
-      <c r="P12" s="55"/>
-      <c r="Q12" s="55"/>
-      <c r="R12" s="55"/>
+      <c r="K12" s="71"/>
+      <c r="L12" s="71"/>
+      <c r="M12" s="71"/>
+      <c r="N12" s="71"/>
+      <c r="O12" s="71"/>
+      <c r="P12" s="71"/>
+      <c r="Q12" s="71"/>
+      <c r="R12" s="71"/>
       <c r="S12" s="9"/>
     </row>
     <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="48" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
+      <c r="A13" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
       <c r="D13" s="47" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>15</v>
@@ -1425,11 +1472,11 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
+      <c r="A14" s="74" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="75"/>
+      <c r="C14" s="76"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1460,11 +1507,11 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="57"/>
-      <c r="C15" s="57"/>
+      <c r="A15" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="75"/>
+      <c r="C15" s="76"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1495,11 +1542,11 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
+      <c r="A16" s="74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="75"/>
+      <c r="C16" s="76"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1530,11 +1577,11 @@
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="57" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="57"/>
-      <c r="C17" s="57"/>
+      <c r="A17" s="74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="75"/>
+      <c r="C17" s="76"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1565,11 +1612,11 @@
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
+      <c r="A18" s="74" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="76"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1600,11 +1647,11 @@
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="57"/>
-      <c r="C19" s="57"/>
+      <c r="A19" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="75"/>
+      <c r="C19" s="76"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1635,11 +1682,11 @@
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="57"/>
-      <c r="C20" s="57"/>
+      <c r="A20" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="75"/>
+      <c r="C20" s="76"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -1670,11 +1717,11 @@
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="57" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="57"/>
-      <c r="C21" s="57"/>
+      <c r="A21" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="75"/>
+      <c r="C21" s="76"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -1705,18 +1752,18 @@
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A22" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="B22" s="57"/>
-      <c r="C22" s="57"/>
+      <c r="A22" s="74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="75"/>
+      <c r="C22" s="76"/>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
       <c r="F22" s="15"/>
       <c r="G22" s="15"/>
       <c r="H22" s="15"/>
       <c r="I22" s="16">
-        <f t="shared" si="1"/>
+        <f>+SUM(D22:H22)</f>
         <v>0</v>
       </c>
       <c r="J22" s="17"/>
@@ -1725,26 +1772,26 @@
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="18">
-        <f t="shared" si="0"/>
+        <f>+$O$4*(J22+K22-N22)</f>
         <v>0</v>
       </c>
       <c r="P22" s="17"/>
       <c r="Q22" s="17">
-        <f t="shared" si="2"/>
+        <f>+J22+K22+L22+M22+O22+P22</f>
         <v>0</v>
       </c>
       <c r="R22" s="18"/>
       <c r="S22" s="18">
-        <f t="shared" si="3"/>
+        <f>+Q22-R22</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A23" s="57" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
+      <c r="A23" s="59" t="s">
+        <v>43</v>
+      </c>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -1775,11 +1822,11 @@
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A24" s="58" t="s">
+      <c r="A24" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
+      <c r="B24" s="63"/>
+      <c r="C24" s="63"/>
       <c r="D24" s="15">
         <f>SUM(D14:D23)</f>
         <v>0</v>
@@ -1900,24 +1947,24 @@
       <c r="S27" s="31"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="62" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="56"/>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
-      <c r="E28" s="56"/>
-      <c r="F28" s="56"/>
-      <c r="G28" s="56"/>
-      <c r="H28" s="56"/>
-      <c r="I28" s="56"/>
-      <c r="J28" s="56"/>
-      <c r="K28" s="56"/>
-      <c r="L28" s="56"/>
-      <c r="M28" s="56"/>
-      <c r="N28" s="56"/>
-      <c r="O28" s="56"/>
-      <c r="P28" s="56"/>
+      <c r="B28" s="62"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="62"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="62"/>
+      <c r="N28" s="62"/>
+      <c r="O28" s="62"/>
+      <c r="P28" s="62"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" s="32"/>
@@ -1958,95 +2005,95 @@
       <c r="P30" s="32"/>
     </row>
     <row r="31" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="59" t="str">
+      <c r="A31" s="55" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
-        <v xml:space="preserve">participant </v>
-      </c>
-      <c r="B31" s="60"/>
+        <v>participant ETF</v>
+      </c>
+      <c r="B31" s="56"/>
       <c r="C31" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="57" t="s">
+      <c r="D31" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="61"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="61"/>
-      <c r="P31" s="61"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
+      <c r="L31" s="60"/>
+      <c r="M31" s="60"/>
+      <c r="N31" s="60"/>
+      <c r="O31" s="60"/>
+      <c r="P31" s="60"/>
     </row>
     <row r="32" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="62" t="s">
+      <c r="A32" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="62"/>
+      <c r="B32" s="49"/>
       <c r="C32" s="34"/>
-      <c r="D32" s="63" t="s">
-        <v>67</v>
-      </c>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
+      <c r="D32" s="61" t="s">
+        <v>59</v>
+      </c>
+      <c r="E32" s="54"/>
+      <c r="F32" s="54"/>
+      <c r="G32" s="54"/>
+      <c r="H32" s="54"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="54"/>
+      <c r="K32" s="54"/>
+      <c r="L32" s="54"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="54"/>
+      <c r="P32" s="54"/>
       <c r="S32" s="31"/>
     </row>
     <row r="33" spans="1:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="62" t="s">
+      <c r="A33" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="62"/>
+      <c r="B33" s="49"/>
       <c r="C33" s="35"/>
-      <c r="D33" s="64" t="s">
-        <v>68</v>
-      </c>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
-      <c r="P33" s="64"/>
+      <c r="D33" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="E33" s="54"/>
+      <c r="F33" s="54"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="54"/>
+      <c r="I33" s="54"/>
+      <c r="J33" s="54"/>
+      <c r="K33" s="54"/>
+      <c r="L33" s="54"/>
+      <c r="M33" s="54"/>
+      <c r="N33" s="54"/>
+      <c r="O33" s="54"/>
+      <c r="P33" s="54"/>
       <c r="S33" s="31"/>
     </row>
     <row r="34" spans="1:19" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="62" t="s">
+      <c r="A34" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="62"/>
+      <c r="B34" s="49"/>
       <c r="C34" s="35"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="64"/>
-      <c r="F34" s="64"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="64"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="64"/>
-      <c r="N34" s="64"/>
-      <c r="O34" s="64"/>
-      <c r="P34" s="64"/>
+      <c r="D34" s="54"/>
+      <c r="E34" s="54"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="54"/>
+      <c r="L34" s="54"/>
+      <c r="M34" s="54"/>
+      <c r="N34" s="54"/>
+      <c r="O34" s="54"/>
+      <c r="P34" s="54"/>
       <c r="S34" s="31"/>
     </row>
     <row r="35" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
@@ -2080,97 +2127,97 @@
       <c r="P36" s="38"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A37" s="59" t="str">
+      <c r="A37" s="55" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B37" s="60"/>
+      <c r="B37" s="56"/>
       <c r="C37" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="69" t="s">
+      <c r="D37" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="70"/>
-      <c r="P37" s="70"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
     </row>
     <row r="38" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="62" t="s">
+      <c r="A38" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="62"/>
+      <c r="B38" s="49"/>
       <c r="C38" s="35"/>
-      <c r="D38" s="68" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" s="64"/>
-      <c r="F38" s="64"/>
-      <c r="G38" s="64"/>
-      <c r="H38" s="64"/>
-      <c r="I38" s="64"/>
-      <c r="J38" s="64"/>
-      <c r="K38" s="64"/>
-      <c r="L38" s="64"/>
-      <c r="M38" s="64"/>
-      <c r="N38" s="64"/>
-      <c r="O38" s="64"/>
-      <c r="P38" s="64"/>
+      <c r="D38" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="54"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="54"/>
+      <c r="L38" s="54"/>
+      <c r="M38" s="54"/>
+      <c r="N38" s="54"/>
+      <c r="O38" s="54"/>
+      <c r="P38" s="54"/>
       <c r="S38" s="31"/>
     </row>
     <row r="39" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="62" t="s">
+      <c r="A39" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="62"/>
+      <c r="B39" s="49"/>
       <c r="C39" s="35"/>
-      <c r="D39" s="65" t="s">
+      <c r="D39" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="66"/>
-      <c r="F39" s="66"/>
-      <c r="G39" s="66"/>
-      <c r="H39" s="66"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="66"/>
-      <c r="K39" s="66"/>
-      <c r="L39" s="66"/>
-      <c r="M39" s="66"/>
-      <c r="N39" s="66"/>
-      <c r="O39" s="66"/>
-      <c r="P39" s="67"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="51"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="51"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="51"/>
+      <c r="M39" s="51"/>
+      <c r="N39" s="51"/>
+      <c r="O39" s="51"/>
+      <c r="P39" s="52"/>
       <c r="S39" s="31"/>
     </row>
     <row r="40" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="62" t="s">
+      <c r="A40" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="62"/>
+      <c r="B40" s="49"/>
       <c r="C40" s="35"/>
-      <c r="D40" s="68" t="s">
+      <c r="D40" s="53" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="64"/>
-      <c r="F40" s="64"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="64"/>
-      <c r="I40" s="64"/>
-      <c r="J40" s="64"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="64"/>
-      <c r="N40" s="64"/>
-      <c r="O40" s="64"/>
-      <c r="P40" s="64"/>
+      <c r="E40" s="54"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="54"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="54"/>
+      <c r="K40" s="54"/>
+      <c r="L40" s="54"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="54"/>
+      <c r="O40" s="54"/>
+      <c r="P40" s="54"/>
       <c r="S40" s="31"/>
     </row>
   </sheetData>
@@ -2178,34 +2225,15 @@
     <protectedRange sqref="J14:N23 C32:P40 D14:H23 P14:P23 R14:S23 O6" name="Range1"/>
   </protectedRanges>
   <mergeCells count="41">
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="D39:P39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="D40:P40"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="D34:P34"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:P38"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:P32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:P33"/>
-    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A15:C15"/>
     <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="E4:I4"/>
@@ -2219,6 +2247,25 @@
     <mergeCell ref="A10:R10"/>
     <mergeCell ref="D12:I12"/>
     <mergeCell ref="J12:R12"/>
+    <mergeCell ref="A28:P28"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:P32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:P33"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="D39:P39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="D40:P40"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="D34:P34"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:P38"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -2241,8 +2288,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2253,10 +2300,10 @@
   <sheetData>
     <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="72"/>
+      <c r="B2" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="73"/>
       <c r="D2" s="43">
         <f>SUM(P5:P35)</f>
         <v>0</v>
@@ -2264,22 +2311,22 @@
     </row>
     <row r="4" spans="2:16" ht="162" x14ac:dyDescent="0.3">
       <c r="B4" s="41" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D4" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="44" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="40" t="s">
+      <c r="G4" s="44" t="s">
         <v>55</v>
-      </c>
-      <c r="F4" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>63</v>
       </c>
       <c r="H4" s="10" t="s">
         <v>13</v>
@@ -2297,21 +2344,21 @@
         <v>17</v>
       </c>
       <c r="M4" s="45" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="O4" s="10" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="P4" s="46" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B5" s="39" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
@@ -2332,7 +2379,9 @@
       </c>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="39"/>
+      <c r="B6" s="39" t="s">
+        <v>65</v>
+      </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
@@ -2352,7 +2401,9 @@
       </c>
     </row>
     <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="39"/>
+      <c r="B7" s="39" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
@@ -2372,7 +2423,9 @@
       </c>
     </row>
     <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="39"/>
+      <c r="B8" s="39" t="s">
+        <v>67</v>
+      </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
@@ -2392,7 +2445,9 @@
       </c>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="39"/>
+      <c r="B9" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
@@ -2412,7 +2467,9 @@
       </c>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="39"/>
+      <c r="B10" s="39" t="s">
+        <v>69</v>
+      </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
@@ -2432,7 +2489,9 @@
       </c>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="39"/>
+      <c r="B11" s="39" t="s">
+        <v>70</v>
+      </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
@@ -2452,7 +2511,9 @@
       </c>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="39"/>
+      <c r="B12" s="39" t="s">
+        <v>71</v>
+      </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
@@ -2944,7 +3005,7 @@
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B5" sqref="B5:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2958,10 +3019,10 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="72"/>
+      <c r="B2" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="73"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
         <v>0</v>
@@ -2969,32 +3030,34 @@
     </row>
     <row r="4" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="41" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
+      <c r="B5" s="39" t="s">
+        <v>64</v>
+      </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
@@ -3007,7 +3070,9 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="39"/>
+      <c r="B6" s="39" t="s">
+        <v>65</v>
+      </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
@@ -3020,7 +3085,9 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="39"/>
+      <c r="B7" s="39" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
@@ -3033,7 +3100,9 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="39"/>
+      <c r="B8" s="39" t="s">
+        <v>67</v>
+      </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
@@ -3046,7 +3115,9 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="39"/>
+      <c r="B9" s="39" t="s">
+        <v>68</v>
+      </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
@@ -3059,7 +3130,9 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="39"/>
+      <c r="B10" s="39" t="s">
+        <v>69</v>
+      </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
@@ -3072,7 +3145,9 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="39"/>
+      <c r="B11" s="39" t="s">
+        <v>70</v>
+      </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
@@ -3085,7 +3160,9 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="39"/>
+      <c r="B12" s="39" t="s">
+        <v>71</v>
+      </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
@@ -3409,7 +3486,7 @@
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3423,10 +3500,10 @@
   <sheetData>
     <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="72"/>
+      <c r="B2" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="73"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
         <v>0</v>
@@ -3434,32 +3511,34 @@
     </row>
     <row r="4" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="41" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C4" s="41" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="H4" s="40" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="39"/>
+      <c r="B5" s="48" t="s">
+        <v>64</v>
+      </c>
       <c r="C5" s="39"/>
       <c r="D5" s="39"/>
       <c r="E5" s="39"/>
@@ -3472,7 +3551,9 @@
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="39"/>
+      <c r="B6" s="48" t="s">
+        <v>65</v>
+      </c>
       <c r="C6" s="39"/>
       <c r="D6" s="39"/>
       <c r="E6" s="39"/>
@@ -3485,7 +3566,9 @@
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="39"/>
+      <c r="B7" s="48" t="s">
+        <v>66</v>
+      </c>
       <c r="C7" s="39"/>
       <c r="D7" s="39"/>
       <c r="E7" s="39"/>
@@ -3498,7 +3581,9 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="39"/>
+      <c r="B8" s="48" t="s">
+        <v>67</v>
+      </c>
       <c r="C8" s="39"/>
       <c r="D8" s="39"/>
       <c r="E8" s="39"/>
@@ -3511,7 +3596,9 @@
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="39"/>
+      <c r="B9" s="48" t="s">
+        <v>68</v>
+      </c>
       <c r="C9" s="39"/>
       <c r="D9" s="39"/>
       <c r="E9" s="39"/>
@@ -3524,7 +3611,9 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="39"/>
+      <c r="B10" s="48" t="s">
+        <v>69</v>
+      </c>
       <c r="C10" s="39"/>
       <c r="D10" s="39"/>
       <c r="E10" s="39"/>
@@ -3537,7 +3626,9 @@
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="39"/>
+      <c r="B11" s="48" t="s">
+        <v>70</v>
+      </c>
       <c r="C11" s="39"/>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
@@ -3550,7 +3641,9 @@
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="39"/>
+      <c r="B12" s="48" t="s">
+        <v>71</v>
+      </c>
       <c r="C12" s="39"/>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>

</xml_diff>

<commit_message>
Uradio prvu tabelu i travel troskove
</commit_message>
<xml_diff>
--- a/2b Format partner budget - Horizon2020.xlsx
+++ b/2b Format partner budget - Horizon2020.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Anja\Fakultet\6. semestar\USP\Projekat\Projekat\Projekat_Faza1_ver1\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9189" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Detaljno budzet" sheetId="1" r:id="rId1"/>
@@ -17,7 +12,11 @@
     <sheet name="Equipment - budzet" sheetId="3" r:id="rId3"/>
     <sheet name="Subcontracting - budzet" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Travel - budzet'!$B$4:$P$48</definedName>
+  </definedNames>
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -31,42 +30,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Kampen, Jan-Joris van</author>
-  </authors>
-  <commentList>
-    <comment ref="O13" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Kampen, Jan-Joris van:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Contributions of third parties to be budgeted as personell costs or other direct costs. No indirect costs on these costs when NOT used on the premises of the benificiary.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="106">
   <si>
     <t>Partner budget Horizon 2020</t>
   </si>
@@ -309,16 +274,91 @@
   </si>
   <si>
     <t>ETF</t>
+  </si>
+  <si>
+    <t>АUEB</t>
+  </si>
+  <si>
+    <t>VIZLORE</t>
+  </si>
+  <si>
+    <t>BOSCH</t>
+  </si>
+  <si>
+    <t>LDA</t>
+  </si>
+  <si>
+    <t>VITO</t>
+  </si>
+  <si>
+    <t>FBOX</t>
+  </si>
+  <si>
+    <t>Univerzitet u Beogradu, Elektrotehnički fakultet</t>
+  </si>
+  <si>
+    <t>Athens University Of Economics And Business - Research Center</t>
+  </si>
+  <si>
+    <t>Fondacija Vizlore Labs</t>
+  </si>
+  <si>
+    <t>FundingBox Accelerator Sp. z o.o.</t>
+  </si>
+  <si>
+    <t>Bosch Thermotechnik GmbH</t>
+  </si>
+  <si>
+    <t>Schneider Electric Portugal Lda</t>
+  </si>
+  <si>
+    <t>Vlaamse Instelling voor Technologisch Onderzoek N.V.</t>
+  </si>
+  <si>
+    <t>SRB</t>
+  </si>
+  <si>
+    <t>POL</t>
+  </si>
+  <si>
+    <t>GER</t>
+  </si>
+  <si>
+    <t>POR</t>
+  </si>
+  <si>
+    <t>NED</t>
+  </si>
+  <si>
+    <t>Belgrade</t>
+  </si>
+  <si>
+    <t>Warsaw</t>
+  </si>
+  <si>
+    <t>Stuttgart</t>
+  </si>
+  <si>
+    <t>Lisbon</t>
+  </si>
+  <si>
+    <t>Amsterdam</t>
+  </si>
+  <si>
+    <t>Athens</t>
+  </si>
+  <si>
+    <t>GRE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,19 +423,6 @@
     </font>
     <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -417,8 +444,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,8 +512,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -658,12 +703,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -744,17 +817,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -767,13 +840,50 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -796,56 +906,31 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -893,7 +978,7 @@
         <xdr:cNvPr id="3" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{DA4F558B-8D56-430D-AA83-772AD1DE26DE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -905,7 +990,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -928,14 +1013,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -995,7 +1080,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1027,10 +1112,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1062,7 +1146,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1238,17 +1321,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:T38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.65"/>
   <cols>
     <col min="1" max="1" width="11.44140625" customWidth="1"/>
     <col min="2" max="2" width="24.77734375" customWidth="1"/>
@@ -1263,77 +1346,77 @@
     <col min="15" max="19" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="25.05">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E3" s="53"/>
-      <c r="F3" s="53"/>
-      <c r="G3" s="53"/>
-      <c r="H3" s="53"/>
-      <c r="I3" s="53"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19">
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+    </row>
+    <row r="4" spans="1:19">
       <c r="D4" s="2"/>
-      <c r="E4" s="54" t="s">
+      <c r="E4" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
       <c r="J4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="L4" s="55" t="s">
+      <c r="L4" s="68" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
       <c r="O4" s="4">
         <v>0.25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19">
       <c r="D5" s="2"/>
-      <c r="E5" s="54" t="s">
+      <c r="E5" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
       <c r="J5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="L5" s="55" t="s">
+      <c r="L5" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="M5" s="55"/>
-      <c r="N5" s="55"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
       <c r="O5" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19">
       <c r="D6" s="2"/>
-      <c r="E6" s="54" t="s">
+      <c r="E6" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
       <c r="J6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="L6" s="55" t="s">
+      <c r="L6" s="68" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="55"/>
-      <c r="N6" s="55"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
       <c r="O6" s="5">
         <v>0.7</v>
       </c>
@@ -1342,80 +1425,80 @@
       </c>
       <c r="Q6" s="6"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="E7" s="55" t="s">
+    <row r="7" spans="1:19">
+      <c r="E7" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="55"/>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
       <c r="J7" s="3"/>
-      <c r="L7" s="55" t="s">
+      <c r="L7" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="M7" s="55"/>
-      <c r="N7" s="55"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
       <c r="O7" s="4">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19">
       <c r="J8" s="2"/>
       <c r="O8" s="7"/>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="10" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="56" t="s">
+    <row r="9" spans="1:19" ht="15.25" thickBot="1"/>
+    <row r="10" spans="1:19" ht="16.5" thickBot="1">
+      <c r="A10" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
-      <c r="P10" s="57"/>
-      <c r="Q10" s="57"/>
-      <c r="R10" s="57"/>
+      <c r="B10" s="70"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="70"/>
+      <c r="G10" s="70"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="70"/>
+      <c r="L10" s="70"/>
+      <c r="M10" s="70"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="70"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="70"/>
+      <c r="R10" s="70"/>
       <c r="S10" s="8"/>
     </row>
-    <row r="12" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D12" s="58" t="s">
+    <row r="12" spans="1:19" ht="15.9">
+      <c r="D12" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="59" t="s">
+      <c r="E12" s="71"/>
+      <c r="F12" s="71"/>
+      <c r="G12" s="71"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="72" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="59"/>
-      <c r="L12" s="59"/>
-      <c r="M12" s="59"/>
-      <c r="N12" s="59"/>
-      <c r="O12" s="59"/>
-      <c r="P12" s="59"/>
-      <c r="Q12" s="59"/>
-      <c r="R12" s="59"/>
+      <c r="K12" s="72"/>
+      <c r="L12" s="72"/>
+      <c r="M12" s="72"/>
+      <c r="N12" s="72"/>
+      <c r="O12" s="72"/>
+      <c r="P12" s="72"/>
+      <c r="Q12" s="72"/>
+      <c r="R12" s="72"/>
       <c r="S12" s="9"/>
     </row>
-    <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="52" t="s">
+    <row r="13" spans="1:19" s="14" customFormat="1" ht="90" customHeight="1">
+      <c r="A13" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="52"/>
-      <c r="C13" s="52"/>
+      <c r="B13" s="65"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="47" t="s">
         <v>60</v>
       </c>
@@ -1465,12 +1548,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A14" s="49" t="s">
+    <row r="14" spans="1:19">
+      <c r="A14" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
+      <c r="B14" s="74"/>
+      <c r="C14" s="75"/>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
@@ -1500,12 +1583,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A15" s="49" t="s">
+    <row r="15" spans="1:19">
+      <c r="A15" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
+      <c r="B15" s="74"/>
+      <c r="C15" s="75"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
@@ -1535,12 +1618,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="49" t="s">
+    <row r="16" spans="1:19">
+      <c r="A16" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="50"/>
-      <c r="C16" s="51"/>
+      <c r="B16" s="74"/>
+      <c r="C16" s="75"/>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
@@ -1570,12 +1653,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A17" s="49" t="s">
+    <row r="17" spans="1:20">
+      <c r="A17" s="73" t="s">
         <v>73</v>
       </c>
-      <c r="B17" s="50"/>
-      <c r="C17" s="51"/>
+      <c r="B17" s="74"/>
+      <c r="C17" s="75"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -1605,12 +1688,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A18" s="49" t="s">
+    <row r="18" spans="1:20">
+      <c r="A18" s="73" t="s">
         <v>74</v>
       </c>
-      <c r="B18" s="50"/>
-      <c r="C18" s="51"/>
+      <c r="B18" s="74"/>
+      <c r="C18" s="75"/>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
@@ -1640,12 +1723,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="49" t="s">
+    <row r="19" spans="1:20">
+      <c r="A19" s="73" t="s">
         <v>75</v>
       </c>
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
+      <c r="B19" s="74"/>
+      <c r="C19" s="75"/>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1675,12 +1758,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A20" s="49" t="s">
+    <row r="20" spans="1:20">
+      <c r="A20" s="73" t="s">
         <v>76</v>
       </c>
-      <c r="B20" s="50"/>
-      <c r="C20" s="51"/>
+      <c r="B20" s="74"/>
+      <c r="C20" s="75"/>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
@@ -1710,12 +1793,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A21" s="49" t="s">
+    <row r="21" spans="1:20">
+      <c r="A21" s="73" t="s">
         <v>77</v>
       </c>
-      <c r="B21" s="50"/>
-      <c r="C21" s="51"/>
+      <c r="B21" s="74"/>
+      <c r="C21" s="75"/>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
@@ -1745,79 +1828,79 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20">
       <c r="A22" s="62" t="s">
         <v>18</v>
       </c>
       <c r="B22" s="62"/>
       <c r="C22" s="62"/>
       <c r="D22" s="15">
-        <f>SUM(D14:D21)</f>
+        <f t="shared" ref="D22:S22" si="4">SUM(D14:D21)</f>
         <v>0</v>
       </c>
       <c r="E22" s="15">
-        <f>SUM(E14:E21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F22" s="15">
-        <f>SUM(F14:F21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G22" s="15">
-        <f>SUM(G14:G21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="H22" s="15">
-        <f>SUM(H14:H21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I22" s="19">
-        <f>SUM(I14:I21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J22" s="20">
-        <f>SUM(J14:J21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K22" s="20">
-        <f>SUM(K14:K21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L22" s="20">
-        <f>SUM(L14:L21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M22" s="20">
-        <f>SUM(M14:M21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N22" s="20">
-        <f>SUM(N14:N21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O22" s="20">
-        <f>SUM(O14:O21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P22" s="20">
-        <f>SUM(P14:P21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="Q22" s="20">
-        <f>SUM(Q14:Q21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="R22" s="21">
-        <f>SUM(R14:R21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="S22" s="22">
-        <f>SUM(S14:S21)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T22" s="23"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20">
       <c r="A23" s="24"/>
       <c r="B23" s="24"/>
       <c r="C23" s="24"/>
@@ -1839,7 +1922,7 @@
       <c r="S23" s="23"/>
       <c r="T23" s="23"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20">
       <c r="A24" s="24"/>
       <c r="B24" s="24"/>
       <c r="C24" s="24"/>
@@ -1866,31 +1949,31 @@
       <c r="S24" s="23"/>
       <c r="T24" s="23"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20">
       <c r="A25" s="30"/>
       <c r="S25" s="31"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="60" t="s">
+    <row r="26" spans="1:20">
+      <c r="A26" s="61" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="60"/>
-      <c r="H26" s="60"/>
-      <c r="I26" s="60"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="60"/>
-      <c r="L26" s="60"/>
-      <c r="M26" s="60"/>
-      <c r="N26" s="60"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="60"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="61"/>
+      <c r="L26" s="61"/>
+      <c r="M26" s="61"/>
+      <c r="N26" s="61"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="61"/>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -1908,7 +1991,7 @@
       <c r="O27" s="32"/>
       <c r="P27" s="32"/>
     </row>
-    <row r="28" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="41.2" customHeight="1">
       <c r="A28" s="32" t="s">
         <v>31</v>
       </c>
@@ -1928,99 +2011,99 @@
       <c r="O28" s="32"/>
       <c r="P28" s="32"/>
     </row>
-    <row r="29" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="63" t="str">
+    <row r="29" spans="1:20" ht="41.2" customHeight="1">
+      <c r="A29" s="53" t="str">
         <f>CONCATENATE("participant"," ",J6)</f>
         <v>participant ETF</v>
       </c>
-      <c r="B29" s="64"/>
+      <c r="B29" s="54"/>
       <c r="C29" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="61" t="s">
+      <c r="D29" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="E29" s="65"/>
-      <c r="F29" s="65"/>
-      <c r="G29" s="65"/>
-      <c r="H29" s="65"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="65"/>
-      <c r="K29" s="65"/>
-      <c r="L29" s="65"/>
-      <c r="M29" s="65"/>
-      <c r="N29" s="65"/>
-      <c r="O29" s="65"/>
-      <c r="P29" s="65"/>
-    </row>
-    <row r="30" spans="1:20" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="66" t="s">
+      <c r="E29" s="64"/>
+      <c r="F29" s="64"/>
+      <c r="G29" s="64"/>
+      <c r="H29" s="64"/>
+      <c r="I29" s="64"/>
+      <c r="J29" s="64"/>
+      <c r="K29" s="64"/>
+      <c r="L29" s="64"/>
+      <c r="M29" s="64"/>
+      <c r="N29" s="64"/>
+      <c r="O29" s="64"/>
+      <c r="P29" s="64"/>
+    </row>
+    <row r="30" spans="1:20" ht="36" customHeight="1">
+      <c r="A30" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="66"/>
+      <c r="B30" s="50"/>
       <c r="C30" s="34"/>
-      <c r="D30" s="67" t="s">
+      <c r="D30" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="68"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="68"/>
-      <c r="H30" s="68"/>
-      <c r="I30" s="68"/>
-      <c r="J30" s="68"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="68"/>
-      <c r="M30" s="68"/>
-      <c r="N30" s="68"/>
-      <c r="O30" s="68"/>
-      <c r="P30" s="68"/>
+      <c r="E30" s="52"/>
+      <c r="F30" s="52"/>
+      <c r="G30" s="52"/>
+      <c r="H30" s="52"/>
+      <c r="I30" s="52"/>
+      <c r="J30" s="52"/>
+      <c r="K30" s="52"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="52"/>
+      <c r="P30" s="52"/>
       <c r="S30" s="31"/>
     </row>
-    <row r="31" spans="1:20" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="66" t="s">
+    <row r="31" spans="1:20" ht="29.3" customHeight="1">
+      <c r="A31" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="66"/>
+      <c r="B31" s="50"/>
       <c r="C31" s="35"/>
-      <c r="D31" s="68" t="s">
+      <c r="D31" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="E31" s="68"/>
-      <c r="F31" s="68"/>
-      <c r="G31" s="68"/>
-      <c r="H31" s="68"/>
-      <c r="I31" s="68"/>
-      <c r="J31" s="68"/>
-      <c r="K31" s="68"/>
-      <c r="L31" s="68"/>
-      <c r="M31" s="68"/>
-      <c r="N31" s="68"/>
-      <c r="O31" s="68"/>
-      <c r="P31" s="68"/>
+      <c r="E31" s="52"/>
+      <c r="F31" s="52"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="52"/>
+      <c r="O31" s="52"/>
+      <c r="P31" s="52"/>
       <c r="S31" s="31"/>
     </row>
-    <row r="32" spans="1:20" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="66" t="s">
+    <row r="32" spans="1:20" ht="31.6" customHeight="1">
+      <c r="A32" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="66"/>
+      <c r="B32" s="50"/>
       <c r="C32" s="35"/>
-      <c r="D32" s="68"/>
-      <c r="E32" s="68"/>
-      <c r="F32" s="68"/>
-      <c r="G32" s="68"/>
-      <c r="H32" s="68"/>
-      <c r="I32" s="68"/>
-      <c r="J32" s="68"/>
-      <c r="K32" s="68"/>
-      <c r="L32" s="68"/>
-      <c r="M32" s="68"/>
-      <c r="N32" s="68"/>
-      <c r="O32" s="68"/>
-      <c r="P32" s="68"/>
+      <c r="D32" s="52"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="52"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="52"/>
+      <c r="N32" s="52"/>
+      <c r="O32" s="52"/>
+      <c r="P32" s="52"/>
       <c r="S32" s="31"/>
     </row>
-    <row r="33" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" s="36" customFormat="1">
       <c r="D33" s="37"/>
       <c r="E33" s="37"/>
       <c r="F33" s="37"/>
@@ -2035,7 +2118,7 @@
       <c r="O33" s="37"/>
       <c r="P33" s="37"/>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19">
       <c r="D34" s="38"/>
       <c r="E34" s="38"/>
       <c r="F34" s="38"/>
@@ -2050,98 +2133,98 @@
       <c r="O34" s="38"/>
       <c r="P34" s="38"/>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A35" s="63" t="str">
+    <row r="35" spans="1:19">
+      <c r="A35" s="53" t="str">
         <f>CONCATENATE("participant"," ",C9)</f>
         <v xml:space="preserve">participant </v>
       </c>
-      <c r="B35" s="64"/>
+      <c r="B35" s="54"/>
       <c r="C35" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="73" t="s">
+      <c r="D35" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74"/>
-      <c r="I35" s="74"/>
-      <c r="J35" s="74"/>
-      <c r="K35" s="74"/>
-      <c r="L35" s="74"/>
-      <c r="M35" s="74"/>
-      <c r="N35" s="74"/>
-      <c r="O35" s="74"/>
-      <c r="P35" s="74"/>
-    </row>
-    <row r="36" spans="1:19" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="66" t="s">
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="56"/>
+      <c r="K35" s="56"/>
+      <c r="L35" s="56"/>
+      <c r="M35" s="56"/>
+      <c r="N35" s="56"/>
+      <c r="O35" s="56"/>
+      <c r="P35" s="56"/>
+    </row>
+    <row r="36" spans="1:19" ht="27.8" customHeight="1">
+      <c r="A36" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="66"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="35"/>
-      <c r="D36" s="72" t="s">
+      <c r="D36" s="51" t="s">
         <v>59</v>
       </c>
-      <c r="E36" s="68"/>
-      <c r="F36" s="68"/>
-      <c r="G36" s="68"/>
-      <c r="H36" s="68"/>
-      <c r="I36" s="68"/>
-      <c r="J36" s="68"/>
-      <c r="K36" s="68"/>
-      <c r="L36" s="68"/>
-      <c r="M36" s="68"/>
-      <c r="N36" s="68"/>
-      <c r="O36" s="68"/>
-      <c r="P36" s="68"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="52"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="52"/>
+      <c r="N36" s="52"/>
+      <c r="O36" s="52"/>
+      <c r="P36" s="52"/>
       <c r="S36" s="31"/>
     </row>
-    <row r="37" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="66" t="s">
+    <row r="37" spans="1:19" ht="25.5" customHeight="1">
+      <c r="A37" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="66"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="35"/>
-      <c r="D37" s="69" t="s">
+      <c r="D37" s="58" t="s">
         <v>39</v>
       </c>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="70"/>
-      <c r="K37" s="70"/>
-      <c r="L37" s="70"/>
-      <c r="M37" s="70"/>
-      <c r="N37" s="70"/>
-      <c r="O37" s="70"/>
-      <c r="P37" s="71"/>
+      <c r="E37" s="59"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="59"/>
+      <c r="P37" s="60"/>
       <c r="S37" s="31"/>
     </row>
-    <row r="38" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="66" t="s">
+    <row r="38" spans="1:19" ht="26.25" customHeight="1">
+      <c r="A38" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B38" s="66"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="35"/>
-      <c r="D38" s="72" t="s">
+      <c r="D38" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E38" s="68"/>
-      <c r="F38" s="68"/>
-      <c r="G38" s="68"/>
-      <c r="H38" s="68"/>
-      <c r="I38" s="68"/>
-      <c r="J38" s="68"/>
-      <c r="K38" s="68"/>
-      <c r="L38" s="68"/>
-      <c r="M38" s="68"/>
-      <c r="N38" s="68"/>
-      <c r="O38" s="68"/>
-      <c r="P38" s="68"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="52"/>
+      <c r="G38" s="52"/>
+      <c r="H38" s="52"/>
+      <c r="I38" s="52"/>
+      <c r="J38" s="52"/>
+      <c r="K38" s="52"/>
+      <c r="L38" s="52"/>
+      <c r="M38" s="52"/>
+      <c r="N38" s="52"/>
+      <c r="O38" s="52"/>
+      <c r="P38" s="52"/>
       <c r="S38" s="31"/>
     </row>
   </sheetData>
@@ -2149,6 +2232,37 @@
     <protectedRange sqref="D14:H21 C30:P38 P14:P21 R14:S21 O6 J14:N21" name="Range1"/>
   </protectedRanges>
   <mergeCells count="39">
+    <mergeCell ref="D12:I12"/>
+    <mergeCell ref="J12:R12"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="E6:I6"/>
+    <mergeCell ref="L6:N6"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="L7:N7"/>
+    <mergeCell ref="A10:R10"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="A26:P26"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:P29"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:P30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:P31"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:P37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="D38:P38"/>
     <mergeCell ref="A32:B32"/>
@@ -2157,37 +2271,6 @@
     <mergeCell ref="D35:P35"/>
     <mergeCell ref="A36:B36"/>
     <mergeCell ref="D36:P36"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:P30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:P31"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:P37"/>
-    <mergeCell ref="A26:P26"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:P29"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="E6:I6"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="A10:R10"/>
-    <mergeCell ref="D12:I12"/>
-    <mergeCell ref="J12:R12"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <conditionalFormatting sqref="O4">
     <cfRule type="expression" dxfId="0" priority="1">
@@ -2202,36 +2285,38 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
+    <col min="1" max="1" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.5546875" customWidth="1"/>
+    <col min="4" max="4" width="55" customWidth="1"/>
     <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:16" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="75" t="s">
+    <row r="1" spans="1:16" ht="15.25" thickBot="1"/>
+    <row r="2" spans="1:16" ht="18.95" thickBot="1">
+      <c r="B2" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="43">
         <f>SUM(P5:P35)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="2:16" ht="162" x14ac:dyDescent="0.3">
+        <v>118200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="156.19999999999999">
       <c r="B4" s="41" t="s">
         <v>50</v>
       </c>
@@ -2278,638 +2363,1703 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="15.9">
+      <c r="A5" s="78"/>
       <c r="B5" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
+      <c r="C5" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F5" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G5" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H5" s="39">
+        <v>2</v>
+      </c>
       <c r="I5" s="39"/>
       <c r="J5" s="39"/>
       <c r="K5" s="39"/>
       <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
+      <c r="M5" s="39">
+        <v>4</v>
+      </c>
+      <c r="N5" s="39">
+        <v>1200</v>
+      </c>
+      <c r="O5" s="39">
+        <v>1100</v>
+      </c>
       <c r="P5" s="39">
         <f>N5+O5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B6" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A6" s="78"/>
+      <c r="B6" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E6" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G6" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H6" s="39">
+        <v>2</v>
+      </c>
       <c r="I6" s="39"/>
       <c r="J6" s="39"/>
       <c r="K6" s="39"/>
       <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
+      <c r="M6" s="39">
+        <v>4</v>
+      </c>
+      <c r="N6" s="39">
+        <v>1200</v>
+      </c>
+      <c r="O6" s="39">
+        <v>1100</v>
+      </c>
       <c r="P6" s="39">
-        <f t="shared" ref="P6:P35" si="0">N6+O6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B7" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="39"/>
-      <c r="H7" s="39"/>
+        <f t="shared" ref="P6:P48" si="0">N6+O6</f>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A7" s="79"/>
+      <c r="B7" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E7" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G7" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H7" s="39">
+        <v>2</v>
+      </c>
       <c r="I7" s="39"/>
       <c r="J7" s="39"/>
       <c r="K7" s="39"/>
       <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
+      <c r="M7" s="39">
+        <v>4</v>
+      </c>
+      <c r="N7" s="39">
+        <v>1600</v>
+      </c>
+      <c r="O7" s="39">
+        <v>1100</v>
+      </c>
       <c r="P7" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B8" s="39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="39"/>
-      <c r="H8" s="39"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.9">
+      <c r="A8" s="78"/>
+      <c r="B8" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E8" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G8" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H8" s="39">
+        <v>2</v>
+      </c>
       <c r="I8" s="39"/>
       <c r="J8" s="39"/>
       <c r="K8" s="39"/>
       <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
+      <c r="M8" s="39">
+        <v>4</v>
+      </c>
+      <c r="N8" s="39">
+        <v>2000</v>
+      </c>
+      <c r="O8" s="39">
+        <v>1100</v>
+      </c>
       <c r="P8" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B9" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.9">
+      <c r="A9" s="78"/>
+      <c r="B9" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G9" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H9" s="39">
+        <v>2</v>
+      </c>
       <c r="I9" s="39"/>
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
       <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
+      <c r="M9" s="39">
+        <v>4</v>
+      </c>
+      <c r="N9" s="39">
+        <v>2000</v>
+      </c>
+      <c r="O9" s="39">
+        <v>1100</v>
+      </c>
       <c r="P9" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B10" s="39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.9">
+      <c r="A10" s="78"/>
+      <c r="B10" s="49" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="82" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G10" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="H10" s="39">
+        <v>2</v>
+      </c>
       <c r="I10" s="39"/>
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
       <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
+      <c r="M10" s="39">
+        <v>4</v>
+      </c>
+      <c r="N10" s="39">
+        <v>1200</v>
+      </c>
+      <c r="O10" s="39">
+        <v>1100</v>
+      </c>
       <c r="P10" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B11" s="39" t="s">
-        <v>68</v>
-      </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="39"/>
-      <c r="H11" s="39"/>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="18.95" customHeight="1">
+      <c r="A11" s="80"/>
+      <c r="B11" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H11" s="39">
+        <v>2</v>
+      </c>
       <c r="I11" s="39"/>
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
       <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
+      <c r="M11" s="39">
+        <v>5</v>
+      </c>
+      <c r="N11" s="39">
+        <v>1200</v>
+      </c>
+      <c r="O11" s="39">
+        <v>1000</v>
+      </c>
       <c r="P11" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B12" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="39"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.9">
+      <c r="B12" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="83" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="49" t="s">
+        <v>99</v>
+      </c>
       <c r="H12" s="39"/>
       <c r="I12" s="39"/>
       <c r="J12" s="39"/>
       <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
+      <c r="L12" s="39">
+        <v>2</v>
+      </c>
+      <c r="M12" s="39">
+        <v>5</v>
+      </c>
+      <c r="N12" s="39">
+        <v>1200</v>
+      </c>
+      <c r="O12" s="39">
+        <v>1000</v>
+      </c>
       <c r="P12" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.9">
+      <c r="B13" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E13" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F13" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="49" t="s">
+        <v>99</v>
+      </c>
       <c r="H13" s="39"/>
       <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
+      <c r="J13" s="39">
+        <v>3</v>
+      </c>
       <c r="K13" s="39"/>
       <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
+      <c r="M13" s="39">
+        <v>5</v>
+      </c>
+      <c r="N13" s="39">
+        <v>2400</v>
+      </c>
+      <c r="O13" s="39">
+        <v>1500</v>
+      </c>
       <c r="P13" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
+        <v>3900</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.9">
+      <c r="B14" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E14" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G14" s="49" t="s">
+        <v>99</v>
+      </c>
       <c r="H14" s="39"/>
       <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
+      <c r="J14" s="39">
+        <v>3</v>
+      </c>
       <c r="K14" s="39"/>
       <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
+      <c r="M14" s="39">
+        <v>5</v>
+      </c>
+      <c r="N14" s="39">
+        <v>3000</v>
+      </c>
+      <c r="O14" s="39">
+        <v>1500</v>
+      </c>
       <c r="P14" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-      <c r="D15" s="39"/>
-      <c r="E15" s="39"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.9">
+      <c r="B15" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D15" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E15" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G15" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" s="39">
+        <v>1</v>
+      </c>
       <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
+      <c r="J15" s="39">
+        <v>1</v>
+      </c>
       <c r="K15" s="39"/>
       <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="39"/>
-      <c r="O15" s="39"/>
+      <c r="M15" s="39">
+        <v>5</v>
+      </c>
+      <c r="N15" s="39">
+        <v>2000</v>
+      </c>
+      <c r="O15" s="39">
+        <v>1000</v>
+      </c>
       <c r="P15" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.9">
+      <c r="B16" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E16" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="49" t="s">
+        <v>101</v>
+      </c>
       <c r="H16" s="39"/>
       <c r="I16" s="39"/>
-      <c r="J16" s="39"/>
+      <c r="J16" s="39">
+        <v>2</v>
+      </c>
       <c r="K16" s="39"/>
       <c r="L16" s="39"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="39"/>
-      <c r="O16" s="39"/>
+      <c r="M16" s="39">
+        <v>4</v>
+      </c>
+      <c r="N16" s="39">
+        <v>1600</v>
+      </c>
+      <c r="O16" s="39">
+        <v>1500</v>
+      </c>
       <c r="P16" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" ht="15.9">
+      <c r="B17" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E17" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G17" s="49" t="s">
+        <v>101</v>
+      </c>
       <c r="H17" s="39"/>
       <c r="I17" s="39"/>
       <c r="J17" s="39"/>
       <c r="K17" s="39"/>
-      <c r="L17" s="39"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="39"/>
-      <c r="O17" s="39"/>
+      <c r="L17" s="39">
+        <v>2</v>
+      </c>
+      <c r="M17" s="39">
+        <v>4</v>
+      </c>
+      <c r="N17" s="39">
+        <v>1200</v>
+      </c>
+      <c r="O17" s="49">
+        <v>1500</v>
+      </c>
       <c r="P17" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-      <c r="D18" s="39"/>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" ht="15.9">
+      <c r="B18" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F18" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="49" t="s">
+        <v>101</v>
+      </c>
       <c r="H18" s="39"/>
       <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
+      <c r="J18" s="39">
+        <v>2</v>
+      </c>
       <c r="K18" s="39"/>
       <c r="L18" s="39"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="39"/>
-      <c r="O18" s="39"/>
+      <c r="M18" s="39">
+        <v>4</v>
+      </c>
+      <c r="N18" s="39">
+        <v>1600</v>
+      </c>
+      <c r="O18" s="49">
+        <v>1500</v>
+      </c>
       <c r="P18" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-      <c r="D19" s="39"/>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" ht="15.9">
+      <c r="B19" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D19" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E19" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="49" t="s">
+        <v>101</v>
+      </c>
       <c r="H19" s="39"/>
       <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
+      <c r="J19" s="39">
+        <v>2</v>
+      </c>
       <c r="K19" s="39"/>
       <c r="L19" s="39"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="39"/>
+      <c r="M19" s="39">
+        <v>4</v>
+      </c>
+      <c r="N19" s="39">
+        <v>1200</v>
+      </c>
+      <c r="O19" s="49">
+        <v>1500</v>
+      </c>
       <c r="P19" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="39"/>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15.9">
+      <c r="B20" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>101</v>
+      </c>
       <c r="H20" s="39"/>
       <c r="I20" s="39"/>
-      <c r="J20" s="39"/>
+      <c r="J20" s="39">
+        <v>2</v>
+      </c>
       <c r="K20" s="39"/>
       <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="39"/>
-      <c r="O20" s="39"/>
+      <c r="M20" s="39">
+        <v>4</v>
+      </c>
+      <c r="N20" s="39">
+        <v>1600</v>
+      </c>
+      <c r="O20" s="49">
+        <v>1500</v>
+      </c>
       <c r="P20" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="39"/>
-      <c r="F21" s="39"/>
-      <c r="G21" s="39"/>
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="15.9">
+      <c r="B21" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C21" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G21" s="49" t="s">
+        <v>99</v>
+      </c>
       <c r="H21" s="39"/>
       <c r="I21" s="39"/>
-      <c r="J21" s="39"/>
+      <c r="J21" s="39">
+        <v>3</v>
+      </c>
       <c r="K21" s="39"/>
       <c r="L21" s="39"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="39"/>
-      <c r="O21" s="39"/>
+      <c r="M21" s="39">
+        <v>4</v>
+      </c>
+      <c r="N21" s="39">
+        <v>2400</v>
+      </c>
+      <c r="O21" s="39">
+        <v>1700</v>
+      </c>
       <c r="P21" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="15.9">
+      <c r="B22" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G22" s="49" t="s">
+        <v>99</v>
+      </c>
       <c r="H22" s="39"/>
       <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
+      <c r="J22" s="39">
+        <v>3</v>
+      </c>
       <c r="K22" s="39"/>
       <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
-      <c r="O22" s="39"/>
+      <c r="M22" s="39">
+        <v>4</v>
+      </c>
+      <c r="N22" s="39">
+        <v>3000</v>
+      </c>
+      <c r="O22" s="49">
+        <v>1700</v>
+      </c>
       <c r="P22" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="15.9">
+      <c r="B23" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E23" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F23" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G23" s="49" t="s">
+        <v>99</v>
+      </c>
       <c r="H23" s="39"/>
       <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
+      <c r="J23" s="39">
+        <v>3</v>
+      </c>
       <c r="K23" s="39"/>
       <c r="L23" s="39"/>
-      <c r="M23" s="39"/>
-      <c r="N23" s="39"/>
-      <c r="O23" s="39"/>
+      <c r="M23" s="39">
+        <v>4</v>
+      </c>
+      <c r="N23" s="39">
+        <v>3000</v>
+      </c>
+      <c r="O23" s="49">
+        <v>1700</v>
+      </c>
       <c r="P23" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="15.9">
+      <c r="B24" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D24" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E24" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G24" s="49" t="s">
+        <v>99</v>
+      </c>
       <c r="H24" s="39"/>
       <c r="I24" s="39"/>
       <c r="J24" s="39"/>
       <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
-      <c r="M24" s="39"/>
-      <c r="N24" s="39"/>
-      <c r="O24" s="39"/>
+      <c r="L24" s="39">
+        <v>3</v>
+      </c>
+      <c r="M24" s="39">
+        <v>4</v>
+      </c>
+      <c r="N24" s="39">
+        <v>1800</v>
+      </c>
+      <c r="O24" s="49">
+        <v>1700</v>
+      </c>
       <c r="P24" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="39"/>
-      <c r="N25" s="39"/>
-      <c r="O25" s="39"/>
-      <c r="P25" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="39"/>
-      <c r="N26" s="39"/>
-      <c r="O26" s="39"/>
-      <c r="P26" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
-      <c r="M27" s="39"/>
-      <c r="N27" s="39"/>
-      <c r="O27" s="39"/>
-      <c r="P27" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
-      <c r="M28" s="39"/>
-      <c r="N28" s="39"/>
-      <c r="O28" s="39"/>
-      <c r="P28" s="39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B29" s="39"/>
-      <c r="C29" s="39"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="39"/>
-      <c r="F29" s="39"/>
-      <c r="G29" s="39"/>
-      <c r="H29" s="39"/>
-      <c r="I29" s="39"/>
-      <c r="J29" s="39"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="39"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="15.9">
+      <c r="B25" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F25" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49">
+        <v>3</v>
+      </c>
+      <c r="K25" s="49"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="49">
+        <v>4</v>
+      </c>
+      <c r="N25" s="49">
+        <v>2400</v>
+      </c>
+      <c r="O25" s="49">
+        <v>1700</v>
+      </c>
+      <c r="P25" s="49">
+        <f t="shared" ref="P25:P28" si="1">N25+O25</f>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="15.9">
+      <c r="B26" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F26" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G26" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49">
+        <v>3</v>
+      </c>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49">
+        <v>4</v>
+      </c>
+      <c r="N26" s="49">
+        <v>3000</v>
+      </c>
+      <c r="O26" s="49">
+        <v>1700</v>
+      </c>
+      <c r="P26" s="49">
+        <f t="shared" si="1"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="15.9">
+      <c r="B27" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D27" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E27" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F27" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G27" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49">
+        <v>3</v>
+      </c>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49">
+        <v>4</v>
+      </c>
+      <c r="N27" s="49">
+        <v>3000</v>
+      </c>
+      <c r="O27" s="49">
+        <v>1700</v>
+      </c>
+      <c r="P27" s="49">
+        <f t="shared" si="1"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" ht="15.9">
+      <c r="B28" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E28" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G28" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49">
+        <v>3</v>
+      </c>
+      <c r="M28" s="49">
+        <v>4</v>
+      </c>
+      <c r="N28" s="49">
+        <v>1800</v>
+      </c>
+      <c r="O28" s="49">
+        <v>1700</v>
+      </c>
+      <c r="P28" s="49">
+        <f t="shared" si="1"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" ht="15.9">
+      <c r="B29" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E29" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F29" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G29" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49">
+        <v>3</v>
+      </c>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49">
+        <v>4</v>
+      </c>
+      <c r="N29" s="49">
+        <v>2400</v>
+      </c>
+      <c r="O29" s="49">
+        <v>1700</v>
+      </c>
       <c r="P29" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B30" s="39"/>
-      <c r="C30" s="39"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
-      <c r="G30" s="39"/>
-      <c r="H30" s="39"/>
-      <c r="I30" s="39"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-      <c r="N30" s="39"/>
-      <c r="O30" s="39"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="15.9">
+      <c r="B30" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="49" t="s">
+        <v>92</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F30" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G30" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49">
+        <v>3</v>
+      </c>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49">
+        <v>4</v>
+      </c>
+      <c r="N30" s="49">
+        <v>3000</v>
+      </c>
+      <c r="O30" s="49">
+        <v>1700</v>
+      </c>
       <c r="P30" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B31" s="39"/>
-      <c r="C31" s="39"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="39"/>
-      <c r="F31" s="39"/>
-      <c r="G31" s="39"/>
-      <c r="H31" s="39"/>
-      <c r="I31" s="39"/>
-      <c r="J31" s="39"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="39"/>
-      <c r="O31" s="39"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="15.9">
+      <c r="B31" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E31" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F31" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G31" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49">
+        <v>3</v>
+      </c>
+      <c r="K31" s="49"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="49">
+        <v>4</v>
+      </c>
+      <c r="N31" s="49">
+        <v>3000</v>
+      </c>
+      <c r="O31" s="49">
+        <v>1700</v>
+      </c>
       <c r="P31" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B32" s="39"/>
-      <c r="C32" s="39"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="39"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="39"/>
-      <c r="M32" s="39"/>
-      <c r="N32" s="39"/>
-      <c r="O32" s="39"/>
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="15.9">
+      <c r="B32" s="49" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>90</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F32" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G32" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49">
+        <v>3</v>
+      </c>
+      <c r="M32" s="49">
+        <v>4</v>
+      </c>
+      <c r="N32" s="49">
+        <v>1800</v>
+      </c>
+      <c r="O32" s="49">
+        <v>1700</v>
+      </c>
       <c r="P32" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B33" s="39"/>
-      <c r="C33" s="39"/>
-      <c r="D33" s="39"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16" ht="15.9">
+      <c r="B33" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F33" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G33" s="49" t="s">
+        <v>102</v>
+      </c>
       <c r="H33" s="39"/>
       <c r="I33" s="39"/>
-      <c r="J33" s="39"/>
+      <c r="J33" s="39">
+        <v>4</v>
+      </c>
       <c r="K33" s="39"/>
       <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="39"/>
-      <c r="O33" s="39"/>
+      <c r="M33" s="39">
+        <v>5</v>
+      </c>
+      <c r="N33" s="39">
+        <v>4000</v>
+      </c>
+      <c r="O33" s="39">
+        <v>3500</v>
+      </c>
       <c r="P33" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B34" s="39"/>
-      <c r="C34" s="39"/>
-      <c r="D34" s="39"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16" ht="15.9">
+      <c r="B34" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F34" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G34" s="49" t="s">
+        <v>102</v>
+      </c>
       <c r="H34" s="39"/>
       <c r="I34" s="39"/>
-      <c r="J34" s="39"/>
+      <c r="J34" s="39">
+        <v>4</v>
+      </c>
       <c r="K34" s="39"/>
       <c r="L34" s="39"/>
-      <c r="M34" s="39"/>
-      <c r="N34" s="39"/>
-      <c r="O34" s="39"/>
+      <c r="M34" s="39">
+        <v>5</v>
+      </c>
+      <c r="N34" s="39">
+        <v>4000</v>
+      </c>
+      <c r="O34" s="39">
+        <v>3500</v>
+      </c>
       <c r="P34" s="39">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B35" s="39"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="39"/>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16" ht="15.9">
+      <c r="B35" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="G35" s="49" t="s">
+        <v>102</v>
+      </c>
       <c r="H35" s="39"/>
       <c r="I35" s="39"/>
-      <c r="J35" s="39"/>
+      <c r="J35" s="39">
+        <v>4</v>
+      </c>
       <c r="K35" s="39"/>
       <c r="L35" s="39"/>
-      <c r="M35" s="39"/>
-      <c r="N35" s="39"/>
-      <c r="O35" s="39"/>
+      <c r="M35" s="39">
+        <v>5</v>
+      </c>
+      <c r="N35" s="39">
+        <v>2400</v>
+      </c>
+      <c r="O35" s="39">
+        <v>3500</v>
+      </c>
       <c r="P35" s="39">
+        <f t="shared" si="0"/>
+        <v>5900</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16" ht="15.9">
+      <c r="B36" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F36" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G36" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49">
+        <v>4</v>
+      </c>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49">
+        <v>5</v>
+      </c>
+      <c r="N36" s="49">
+        <v>3200</v>
+      </c>
+      <c r="O36" s="49">
+        <v>3500</v>
+      </c>
+      <c r="P36" s="49">
+        <f t="shared" si="0"/>
+        <v>6700</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16" ht="15.9">
+      <c r="B37" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="82" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F37" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G37" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="49">
+        <v>4</v>
+      </c>
+      <c r="M37" s="49">
+        <v>5</v>
+      </c>
+      <c r="N37" s="49">
+        <v>4000</v>
+      </c>
+      <c r="O37" s="49">
+        <v>3500</v>
+      </c>
+      <c r="P37" s="49">
+        <f t="shared" si="0"/>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16" ht="17.7" customHeight="1">
+      <c r="B38" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D38" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="E38" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="49">
+        <v>4</v>
+      </c>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49">
+        <v>5</v>
+      </c>
+      <c r="N38" s="49">
+        <v>4000</v>
+      </c>
+      <c r="O38" s="49">
+        <v>3500</v>
+      </c>
+      <c r="P38" s="49">
+        <f t="shared" si="0"/>
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16" ht="15.9">
+      <c r="B39" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C39" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="D39" s="83" t="s">
+        <v>89</v>
+      </c>
+      <c r="E39" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F39" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49">
+        <v>1</v>
+      </c>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49">
+        <v>1</v>
+      </c>
+      <c r="M39" s="49">
+        <v>4</v>
+      </c>
+      <c r="N39" s="49">
+        <v>2000</v>
+      </c>
+      <c r="O39" s="49">
+        <v>2100</v>
+      </c>
+      <c r="P39" s="49">
+        <f t="shared" si="0"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16" ht="15.9">
+      <c r="B40" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="78" t="s">
+        <v>80</v>
+      </c>
+      <c r="D40" s="49" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="49" t="s">
+        <v>94</v>
+      </c>
+      <c r="F40" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="G40" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49">
+        <v>1</v>
+      </c>
+      <c r="K40" s="49"/>
+      <c r="L40" s="49">
+        <v>1</v>
+      </c>
+      <c r="M40" s="49">
+        <v>4</v>
+      </c>
+      <c r="N40" s="49">
+        <v>2000</v>
+      </c>
+      <c r="O40" s="49">
+        <v>2100</v>
+      </c>
+      <c r="P40" s="49">
+        <f t="shared" si="0"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16" ht="15.9">
+      <c r="B41" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C41" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="49" t="s">
+        <v>91</v>
+      </c>
+      <c r="E41" s="49" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="G41" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49">
+        <v>1</v>
+      </c>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49">
+        <v>1</v>
+      </c>
+      <c r="M41" s="49">
+        <v>4</v>
+      </c>
+      <c r="N41" s="49">
+        <v>1200</v>
+      </c>
+      <c r="O41" s="49">
+        <v>2100</v>
+      </c>
+      <c r="P41" s="49">
+        <f t="shared" si="0"/>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16" ht="15.9">
+      <c r="B42" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C42" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="D42" s="82" t="s">
+        <v>90</v>
+      </c>
+      <c r="E42" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" s="49" t="s">
+        <v>100</v>
+      </c>
+      <c r="G42" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49">
+        <v>1</v>
+      </c>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49">
+        <v>1</v>
+      </c>
+      <c r="M42" s="49">
+        <v>4</v>
+      </c>
+      <c r="N42" s="49">
+        <v>1600</v>
+      </c>
+      <c r="O42" s="49">
+        <v>2100</v>
+      </c>
+      <c r="P42" s="49">
+        <f t="shared" si="0"/>
+        <v>3700</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16" ht="17.7" customHeight="1">
+      <c r="B43" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="E43" s="81" t="s">
+        <v>105</v>
+      </c>
+      <c r="F43" s="49" t="s">
+        <v>104</v>
+      </c>
+      <c r="G43" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49">
+        <v>1</v>
+      </c>
+      <c r="K43" s="49"/>
+      <c r="L43" s="49">
+        <v>1</v>
+      </c>
+      <c r="M43" s="49">
+        <v>4</v>
+      </c>
+      <c r="N43" s="49">
+        <v>2000</v>
+      </c>
+      <c r="O43" s="49">
+        <v>2100</v>
+      </c>
+      <c r="P43" s="49">
+        <f t="shared" si="0"/>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16" ht="15.9">
+      <c r="B44" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="C44" s="78" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="83" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="G44" s="49" t="s">
+        <v>103</v>
+      </c>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49">
+        <v>1</v>
+      </c>
+      <c r="K44" s="49"/>
+      <c r="L44" s="49">
+        <v>1</v>
+      </c>
+      <c r="M44" s="49">
+        <v>4</v>
+      </c>
+      <c r="N44" s="49">
+        <v>1200</v>
+      </c>
+      <c r="O44" s="49">
+        <v>2100</v>
+      </c>
+      <c r="P44" s="49">
+        <f t="shared" si="0"/>
+        <v>3300</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16">
+      <c r="B45" s="49"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+      <c r="F45" s="49"/>
+      <c r="G45" s="49"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="49"/>
+      <c r="M45" s="49"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16">
+      <c r="B46" s="49"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="49"/>
+      <c r="M46" s="49"/>
+      <c r="N46" s="49"/>
+      <c r="O46" s="49"/>
+      <c r="P46" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16">
+      <c r="B47" s="49"/>
+      <c r="C47" s="49"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="49"/>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="49"/>
+      <c r="M47" s="49"/>
+      <c r="N47" s="49"/>
+      <c r="O47" s="49"/>
+      <c r="P47" s="49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16">
+      <c r="B48" s="49"/>
+      <c r="C48" s="49"/>
+      <c r="D48" s="49"/>
+      <c r="E48" s="49"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="49"/>
+      <c r="M48" s="49"/>
+      <c r="N48" s="49"/>
+      <c r="O48" s="49"/>
+      <c r="P48" s="49">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -2923,14 +4073,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
@@ -2939,18 +4089,18 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="75" t="s">
+    <row r="1" spans="2:9" ht="15.25" thickBot="1"/>
+    <row r="2" spans="2:9" ht="18.95" thickBot="1">
+      <c r="B2" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="43.95">
       <c r="B4" s="41" t="s">
         <v>50</v>
       </c>
@@ -2976,7 +4126,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9">
       <c r="B5" s="39" t="s">
         <v>62</v>
       </c>
@@ -2991,7 +4141,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9">
       <c r="B6" s="39" t="s">
         <v>63</v>
       </c>
@@ -3006,7 +4156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9">
       <c r="B7" s="39" t="s">
         <v>64</v>
       </c>
@@ -3021,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9">
       <c r="B8" s="39" t="s">
         <v>65</v>
       </c>
@@ -3036,7 +4186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9">
       <c r="B9" s="39" t="s">
         <v>66</v>
       </c>
@@ -3051,7 +4201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9">
       <c r="B10" s="39" t="s">
         <v>67</v>
       </c>
@@ -3066,7 +4216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9">
       <c r="B11" s="39" t="s">
         <v>68</v>
       </c>
@@ -3081,7 +4231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9">
       <c r="B12" s="39" t="s">
         <v>69</v>
       </c>
@@ -3096,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9">
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -3109,7 +4259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -3122,7 +4272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9">
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -3135,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9">
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -3148,7 +4298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9">
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -3161,7 +4311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
@@ -3174,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -3187,7 +4337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9">
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="39"/>
@@ -3200,7 +4350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9">
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
       <c r="D21" s="39"/>
@@ -3213,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9">
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -3226,7 +4376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9">
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
@@ -3239,7 +4389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9">
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
       <c r="D24" s="39"/>
@@ -3252,7 +4402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9">
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -3265,7 +4415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9">
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
@@ -3278,7 +4428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9">
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
@@ -3291,7 +4441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9">
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
       <c r="D28" s="39"/>
@@ -3304,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9">
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
@@ -3317,7 +4467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9">
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
@@ -3330,7 +4480,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9">
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
@@ -3343,7 +4493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9">
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
@@ -3356,7 +4506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9">
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
@@ -3369,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
@@ -3382,7 +4532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9">
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>
@@ -3404,14 +4554,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:I35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <cols>
     <col min="2" max="2" width="18.5546875" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
@@ -3420,18 +4570,18 @@
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:9" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="75" t="s">
+    <row r="1" spans="2:9" ht="15.25" thickBot="1"/>
+    <row r="2" spans="2:9" ht="18.95" thickBot="1">
+      <c r="B2" s="76" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="76"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="43">
         <f>SUM(I5:I35)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9" ht="43.95">
       <c r="B4" s="41" t="s">
         <v>50</v>
       </c>
@@ -3457,7 +4607,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9">
       <c r="B5" s="48" t="s">
         <v>62</v>
       </c>
@@ -3472,7 +4622,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9">
       <c r="B6" s="48" t="s">
         <v>63</v>
       </c>
@@ -3487,7 +4637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9">
       <c r="B7" s="48" t="s">
         <v>64</v>
       </c>
@@ -3502,7 +4652,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9">
       <c r="B8" s="48" t="s">
         <v>65</v>
       </c>
@@ -3517,7 +4667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9">
       <c r="B9" s="48" t="s">
         <v>66</v>
       </c>
@@ -3532,7 +4682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9">
       <c r="B10" s="48" t="s">
         <v>67</v>
       </c>
@@ -3547,7 +4697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9">
       <c r="B11" s="48" t="s">
         <v>68</v>
       </c>
@@ -3562,7 +4712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9">
       <c r="B12" s="48" t="s">
         <v>69</v>
       </c>
@@ -3577,7 +4727,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9">
       <c r="B13" s="39"/>
       <c r="C13" s="39"/>
       <c r="D13" s="39"/>
@@ -3590,7 +4740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9">
       <c r="B14" s="39"/>
       <c r="C14" s="39"/>
       <c r="D14" s="39"/>
@@ -3603,7 +4753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9">
       <c r="B15" s="39"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
@@ -3616,7 +4766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9">
       <c r="B16" s="39"/>
       <c r="C16" s="39"/>
       <c r="D16" s="39"/>
@@ -3629,7 +4779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9">
       <c r="B17" s="39"/>
       <c r="C17" s="39"/>
       <c r="D17" s="39"/>
@@ -3642,7 +4792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9">
       <c r="B18" s="39"/>
       <c r="C18" s="39"/>
       <c r="D18" s="39"/>
@@ -3655,7 +4805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9">
       <c r="B19" s="39"/>
       <c r="C19" s="39"/>
       <c r="D19" s="39"/>
@@ -3668,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9">
       <c r="B20" s="39"/>
       <c r="C20" s="39"/>
       <c r="D20" s="39"/>
@@ -3681,7 +4831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9">
       <c r="B21" s="39"/>
       <c r="C21" s="39"/>
       <c r="D21" s="39"/>
@@ -3694,7 +4844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9">
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
       <c r="D22" s="39"/>
@@ -3707,7 +4857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9">
       <c r="B23" s="39"/>
       <c r="C23" s="39"/>
       <c r="D23" s="39"/>
@@ -3720,7 +4870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9">
       <c r="B24" s="39"/>
       <c r="C24" s="39"/>
       <c r="D24" s="39"/>
@@ -3733,7 +4883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9">
       <c r="B25" s="39"/>
       <c r="C25" s="39"/>
       <c r="D25" s="39"/>
@@ -3746,7 +4896,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9">
       <c r="B26" s="39"/>
       <c r="C26" s="39"/>
       <c r="D26" s="39"/>
@@ -3759,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9">
       <c r="B27" s="39"/>
       <c r="C27" s="39"/>
       <c r="D27" s="39"/>
@@ -3772,7 +4922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9">
       <c r="B28" s="39"/>
       <c r="C28" s="39"/>
       <c r="D28" s="39"/>
@@ -3785,7 +4935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9">
       <c r="B29" s="39"/>
       <c r="C29" s="39"/>
       <c r="D29" s="39"/>
@@ -3798,7 +4948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9">
       <c r="B30" s="39"/>
       <c r="C30" s="39"/>
       <c r="D30" s="39"/>
@@ -3811,7 +4961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9">
       <c r="B31" s="39"/>
       <c r="C31" s="39"/>
       <c r="D31" s="39"/>
@@ -3824,7 +4974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9">
       <c r="B32" s="39"/>
       <c r="C32" s="39"/>
       <c r="D32" s="39"/>
@@ -3837,7 +4987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9">
       <c r="B33" s="39"/>
       <c r="C33" s="39"/>
       <c r="D33" s="39"/>
@@ -3850,7 +5000,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9">
       <c r="B34" s="39"/>
       <c r="C34" s="39"/>
       <c r="D34" s="39"/>
@@ -3863,7 +5013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9">
       <c r="B35" s="39"/>
       <c r="C35" s="39"/>
       <c r="D35" s="39"/>

</xml_diff>